<commit_message>
Add drilling dialog under user 4  - full depth drilling  - pecking partial retract  - pecking full retract
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Koen\Projecten\Emcoturn 120\edingCNC\cnc_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B41218C6-388A-4200-AAEF-F963BCED7460}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0E43BF-7A57-46E1-8D49-29BA3BB8EFFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1935" yWindow="5130" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -452,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,6 +651,27 @@
         <v>26</v>
       </c>
     </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <f>E42/TAN(RADIANS(E41))</f>
+        <v>1.2618072999578767</v>
+      </c>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>1.2618073000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add facing cycle macro  - created icons for cycles  - moved cycles to user_macro.cnc
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Koen\Projecten\Emcoturn 120\edingCNC\cnc_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA0E43BF-7A57-46E1-8D49-29BA3BB8EFFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EE945C-FABD-4B6C-BF30-B2111D8F8318}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
   <si>
     <t>EdingCNC variables</t>
   </si>
@@ -126,6 +126,96 @@
   </si>
   <si>
     <t>Return value for dlgmsg  1=OK, -1=cancel</t>
+  </si>
+  <si>
+    <t>simple_turning</t>
+  </si>
+  <si>
+    <t>Z1</t>
+  </si>
+  <si>
+    <t>Z2</t>
+  </si>
+  <si>
+    <t>diameter A</t>
+  </si>
+  <si>
+    <t>diameter B</t>
+  </si>
+  <si>
+    <t>depth of cut</t>
+  </si>
+  <si>
+    <t>finish amount</t>
+  </si>
+  <si>
+    <t>Vc [m/s]</t>
+  </si>
+  <si>
+    <t>F [mm/min]</t>
+  </si>
+  <si>
+    <t>Z clearance</t>
+  </si>
+  <si>
+    <t>retract amount</t>
+  </si>
+  <si>
+    <t>roughing complete flag</t>
+  </si>
+  <si>
+    <t>desired cutting depth</t>
+  </si>
+  <si>
+    <t>last cut diameter</t>
+  </si>
+  <si>
+    <t>cycle_driling</t>
+  </si>
+  <si>
+    <t>include tip flag</t>
+  </si>
+  <si>
+    <t>tip angle</t>
+  </si>
+  <si>
+    <t>drill diameter</t>
+  </si>
+  <si>
+    <t>peck depth</t>
+  </si>
+  <si>
+    <t>full retract</t>
+  </si>
+  <si>
+    <t>Fn [mm/rev]</t>
+  </si>
+  <si>
+    <t>drilling spindle speed</t>
+  </si>
+  <si>
+    <t>cutting speed [mm/min]</t>
+  </si>
+  <si>
+    <t>drill tip extension amount</t>
+  </si>
+  <si>
+    <t>cycle_facing</t>
+  </si>
+  <si>
+    <t>Vc [m/min]</t>
+  </si>
+  <si>
+    <t>F cutting speed [mm/min]</t>
+  </si>
+  <si>
+    <t>X clearance</t>
+  </si>
+  <si>
+    <t>desired Z value for cutting</t>
+  </si>
+  <si>
+    <t>1512 last cut Z value</t>
   </si>
 </sst>
 </file>
@@ -161,7 +251,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -169,11 +259,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -181,6 +280,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,34 +565,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E47"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.85546875" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -496,12 +601,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>1200</v>
       </c>
@@ -512,163 +617,647 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>1300</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>1400</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>1401</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="7"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>1402</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>1403</v>
+      </c>
+      <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="7"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>1404</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="7"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>1405</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="7"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>1406</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>1407</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>1408</v>
+      </c>
+      <c r="B16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>1409</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>1410</v>
+      </c>
+      <c r="B18" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>1411</v>
+      </c>
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="5">
+        <v>1412</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="7"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>1450</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="7"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>1451</v>
+      </c>
+      <c r="B22" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="7"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>1452</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="7"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>1453</v>
+      </c>
+      <c r="B24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>1454</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="7"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>1455</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="7"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>1456</v>
+      </c>
+      <c r="B27" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" s="7"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>1457</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>1458</v>
+      </c>
+      <c r="B29" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>1459</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" s="7"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>1460</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="7"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>1461</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>1462</v>
+      </c>
+      <c r="B33" t="s">
+        <v>49</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="5">
+        <v>1463</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>1500</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>1501</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>1502</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>1503</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>1504</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4">
+        <v>1505</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="4">
+        <v>1506</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="4">
+        <v>1507</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="4">
+        <v>1508</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="4">
+        <v>1509</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="4">
+        <v>1510</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="4">
+        <v>1511</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="5">
+        <v>1512</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="4"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="4"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="4"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
         <v>5001</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B53" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
         <v>5002</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B54" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
         <v>5003</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B55" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
         <v>5004</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B56" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
         <v>5005</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B57" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
         <v>5006</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B58" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
         <v>5008</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B59" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
         <v>5009</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B60" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
         <v>5010</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B61" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
         <v>5011</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B62" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
         <v>5012</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B63" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
         <v>5013</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B64" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
         <v>5009</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B65" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>18</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B67" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
         <v>5380</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B68" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
         <v>5398</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B69" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E41">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E86">
         <v>59</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E42">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E87">
         <v>2.1</v>
       </c>
     </row>
-    <row r="45" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E45">
-        <f>E42/TAN(RADIANS(E41))</f>
+    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E90">
+        <f>E87/TAN(RADIANS(E86))</f>
         <v>1.2618072999578767</v>
       </c>
     </row>
-    <row r="47" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E47">
+    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E92">
         <v>1.2618073000000001</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix bug tool 8 in toolchange macro
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Koen\Projecten\Emcoturn 120\edingCNC\cnc_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77EE945C-FABD-4B6C-BF30-B2111D8F8318}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1678178-0AA2-4560-A8AE-54FA074DB5CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
   <si>
     <t>EdingCNC variables</t>
   </si>
@@ -216,6 +216,42 @@
   </si>
   <si>
     <t>1512 last cut Z value</t>
+  </si>
+  <si>
+    <t>max spindle speed</t>
+  </si>
+  <si>
+    <t>diameter</t>
+  </si>
+  <si>
+    <t>vc</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>n = Vc*1000/pi*D</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>mm/rev</t>
+  </si>
+  <si>
+    <t>[rpm]</t>
+  </si>
+  <si>
+    <t>[m/min]</t>
+  </si>
+  <si>
+    <t>[mm]</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>m/min</t>
   </si>
 </sst>
 </file>
@@ -272,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -285,6 +321,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,36 +810,36 @@
       </c>
       <c r="D19" s="7"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
         <v>1412</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
-        <v>1450</v>
-      </c>
-      <c r="B21" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" t="s">
-        <v>41</v>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="5">
+        <v>1413</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D21" s="7"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" t="s">
         <v>41</v>
@@ -811,10 +848,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
@@ -823,10 +860,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
@@ -835,10 +872,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
@@ -847,10 +884,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
@@ -859,10 +896,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="B27" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C27" t="s">
         <v>41</v>
@@ -871,10 +908,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
         <v>41</v>
@@ -883,10 +920,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B29" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
         <v>41</v>
@@ -895,10 +932,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="B30" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C30" t="s">
         <v>41</v>
@@ -907,10 +944,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="B31" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C31" t="s">
         <v>41</v>
@@ -919,10 +956,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
         <v>41</v>
@@ -931,57 +968,58 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="B33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
         <v>41</v>
       </c>
       <c r="D33" s="7"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>1462</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="5">
         <v>1463</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C35" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
-        <v>1500</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="D35" s="7"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C36" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>51</v>
@@ -989,10 +1027,10 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>51</v>
@@ -1000,10 +1038,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>51</v>
@@ -1011,10 +1049,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>51</v>
@@ -1022,10 +1060,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>51</v>
@@ -1033,10 +1071,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>51</v>
@@ -1044,10 +1082,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>51</v>
@@ -1055,10 +1093,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>51</v>
@@ -1066,10 +1104,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>51</v>
@@ -1077,28 +1115,36 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="5">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="4">
+        <v>1511</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="5">
         <v>1512</v>
       </c>
-      <c r="B47" s="9" t="s">
+      <c r="B48" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C47" s="9" t="s">
+      <c r="C48" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
@@ -1113,152 +1159,196 @@
       <c r="A52" s="4"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3">
-        <v>5001</v>
-      </c>
-      <c r="B53" t="s">
-        <v>5</v>
-      </c>
+      <c r="A53" s="4"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="B54" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="B55" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>5004</v>
+        <v>5003</v>
       </c>
       <c r="B56" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>5005</v>
+        <v>5004</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>5006</v>
+        <v>5005</v>
       </c>
       <c r="B58" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>5008</v>
+        <v>5006</v>
       </c>
       <c r="B59" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>5009</v>
+        <v>5008</v>
       </c>
       <c r="B60" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>5010</v>
+        <v>5009</v>
       </c>
       <c r="B61" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="B62" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
+        <v>5012</v>
+      </c>
+      <c r="B64" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
         <v>5013</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B65" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
         <v>5009</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B66" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>18</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
         <v>5380</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B69" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
         <v>5398</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B70" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E86">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>58</v>
+      </c>
+      <c r="D75">
+        <v>30</v>
+      </c>
+      <c r="E75" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E87">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="90" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E90">
-        <f>E87/TAN(RADIANS(E86))</f>
-        <v>1.2618072999578767</v>
-      </c>
-    </row>
-    <row r="92" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E92">
-        <v>1.2618073000000001</v>
+      <c r="D76">
+        <v>140</v>
+      </c>
+      <c r="E76" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>60</v>
+      </c>
+      <c r="D77">
+        <f>D76*1000/(PI()*D75)</f>
+        <v>1485.4461355243566</v>
+      </c>
+      <c r="E77" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>62</v>
+      </c>
+      <c r="D79">
+        <v>0.1</v>
+      </c>
+      <c r="E79" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>67</v>
+      </c>
+      <c r="D81">
+        <f>D79*D77</f>
+        <v>148.54461355243566</v>
+      </c>
+      <c r="E81" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created external threading cycle macro
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Koen\Projecten\Emcoturn 120\edingCNC\cnc_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1678178-0AA2-4560-A8AE-54FA074DB5CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CBE1AB-5CA0-4B30-A11D-BAC860AF3C14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
   <si>
     <t>EdingCNC variables</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>m/min</t>
+  </si>
+  <si>
+    <t>cycle_threading</t>
   </si>
 </sst>
 </file>
@@ -602,10 +605,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E81"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="G83" sqref="G83"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1146,208 +1149,272 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="4"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="4"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="4"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="4"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="10">
+        <v>1550</v>
+      </c>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="10">
+        <v>1551</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="10">
+        <v>1552</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="10">
+        <v>1553</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="10">
+        <v>1554</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="10">
+        <v>1555</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="10">
+        <v>1556</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="10">
+        <v>1557</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="4"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="4"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
         <v>5001</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B60" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
         <v>5002</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B61" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
         <v>5003</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B62" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
         <v>5004</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B63" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
         <v>5005</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B64" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
         <v>5006</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B65" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
         <v>5008</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B66" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
         <v>5009</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B67" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
         <v>5010</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B68" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
         <v>5011</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B69" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
         <v>5012</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B70" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
         <v>5013</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B71" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
         <v>5009</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B72" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>18</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B74" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A69" s="3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
         <v>5380</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B75" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
         <v>5398</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B76" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>58</v>
-      </c>
-      <c r="D75">
-        <v>30</v>
-      </c>
-      <c r="E75" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
-        <v>59</v>
-      </c>
-      <c r="D76">
-        <v>140</v>
-      </c>
-      <c r="E76" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>60</v>
-      </c>
-      <c r="D77">
-        <f>D76*1000/(PI()*D75)</f>
-        <v>1485.4461355243566</v>
-      </c>
-      <c r="E77" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>62</v>
-      </c>
-      <c r="D79">
-        <v>0.1</v>
-      </c>
-      <c r="E79" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="81" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
+        <v>58</v>
+      </c>
+      <c r="D81">
+        <v>30</v>
+      </c>
+      <c r="E81" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>59</v>
+      </c>
+      <c r="D82">
+        <v>140</v>
+      </c>
+      <c r="E82" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>60</v>
+      </c>
+      <c r="D83">
+        <f>D82*1000/(PI()*D81)</f>
+        <v>1485.4461355243566</v>
+      </c>
+      <c r="E83" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>62</v>
+      </c>
+      <c r="D85">
+        <v>0.1</v>
+      </c>
+      <c r="E85" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="87" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
         <v>67</v>
       </c>
-      <c r="D81">
-        <f>D79*D77</f>
+      <c r="D87">
+        <f>D85*D83</f>
         <v>148.54461355243566</v>
       </c>
-      <c r="E81" t="s">
+      <c r="E87" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cycle_OD_turning: - DOC is now actual depth of cut, not diameter cut - feedrate in mm/min now calculated from Vc and diameter, fixed erratic reading of parameter #5070
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Koen\Projecten\Emcoturn 120\edingCNC\cnc_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02CBE1AB-5CA0-4B30-A11D-BAC860AF3C14}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC75677B-D2A0-4ECB-88FF-FF6521A10FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
   <si>
     <t>EdingCNC variables</t>
   </si>
@@ -255,6 +255,9 @@
   </si>
   <si>
     <t>cycle_threading</t>
+  </si>
+  <si>
+    <t>rpm calculation</t>
   </si>
 </sst>
 </file>
@@ -605,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,36 +828,36 @@
       </c>
       <c r="D20" s="7"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
         <v>1413</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="8" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="7"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>1450</v>
-      </c>
-      <c r="B22" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" t="s">
-        <v>41</v>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="5">
+        <v>1414</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>27</v>
       </c>
       <c r="D22" s="7"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
         <v>41</v>
@@ -863,10 +866,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
         <v>41</v>
@@ -875,10 +878,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="B25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
         <v>41</v>
@@ -887,10 +890,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="B26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C26" t="s">
         <v>41</v>
@@ -899,10 +902,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="B27" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C27" t="s">
         <v>41</v>
@@ -911,10 +914,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="B28" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
         <v>41</v>
@@ -923,10 +926,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
         <v>41</v>
@@ -935,10 +938,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C30" t="s">
         <v>41</v>
@@ -947,10 +950,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="B31" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
         <v>41</v>
@@ -959,10 +962,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="B32" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C32" t="s">
         <v>41</v>
@@ -971,10 +974,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C33" t="s">
         <v>41</v>
@@ -983,57 +986,58 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
         <v>41</v>
       </c>
       <c r="D34" s="7"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>1462</v>
+      </c>
+      <c r="B35" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
         <v>1463</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B36" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C36" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
-        <v>1500</v>
-      </c>
-      <c r="B36" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="D36" s="7"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>51</v>
       </c>
+      <c r="D37" s="7"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>51</v>
@@ -1041,10 +1045,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="8" t="s">
         <v>51</v>
@@ -1052,10 +1056,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>51</v>
@@ -1063,10 +1067,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>51</v>
@@ -1074,10 +1078,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>52</v>
+        <v>33</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>51</v>
@@ -1085,10 +1089,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43" s="8" t="s">
         <v>51</v>
@@ -1096,10 +1100,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>51</v>
@@ -1107,10 +1111,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="C45" s="8" t="s">
         <v>51</v>
@@ -1118,10 +1122,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="C46" s="8" t="s">
         <v>51</v>
@@ -1129,38 +1133,40 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C47" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="5">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="4">
+        <v>1511</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="5">
         <v>1512</v>
       </c>
-      <c r="B48" s="9" t="s">
+      <c r="B49" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C48" s="9" t="s">
+      <c r="C49" s="9" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="10">
-        <v>1550</v>
-      </c>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="10">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8" t="s">
@@ -1169,7 +1175,7 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="10">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8" t="s">
@@ -1178,7 +1184,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="10">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8" t="s">
@@ -1187,7 +1193,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="10">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8" t="s">
@@ -1196,7 +1202,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="10">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8" t="s">
@@ -1205,22 +1211,28 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="10">
-        <v>1556</v>
-      </c>
+        <v>1555</v>
+      </c>
+      <c r="B55" s="8"/>
       <c r="C55" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="10">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="C56" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="4"/>
+      <c r="A57" s="10">
+        <v>1557</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
@@ -1229,192 +1241,195 @@
       <c r="A59" s="4"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="3">
-        <v>5001</v>
-      </c>
-      <c r="B60" t="s">
-        <v>5</v>
-      </c>
+      <c r="A60" s="4"/>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>5002</v>
+        <v>5001</v>
       </c>
       <c r="B61" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
-        <v>5003</v>
+        <v>5002</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
-        <v>5004</v>
+        <v>5003</v>
       </c>
       <c r="B63" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>5005</v>
+        <v>5004</v>
       </c>
       <c r="B64" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>5006</v>
+        <v>5005</v>
       </c>
       <c r="B65" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>5008</v>
+        <v>5006</v>
       </c>
       <c r="B66" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <v>5009</v>
+        <v>5008</v>
       </c>
       <c r="B67" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>5010</v>
+        <v>5009</v>
       </c>
       <c r="B68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>5011</v>
+        <v>5010</v>
       </c>
       <c r="B69" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>5012</v>
+        <v>5011</v>
       </c>
       <c r="B70" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <v>5013</v>
+        <v>5012</v>
       </c>
       <c r="B71" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
+        <v>5013</v>
+      </c>
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
         <v>5009</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B73" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>18</v>
       </c>
-      <c r="B74" t="s">
+      <c r="B75" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="3">
-        <v>5380</v>
-      </c>
-      <c r="B75" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
+        <v>5380</v>
+      </c>
+      <c r="B76" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
         <v>5398</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B77" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C81" t="s">
-        <v>58</v>
-      </c>
-      <c r="D81">
-        <v>30</v>
-      </c>
-      <c r="E81" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D82">
-        <v>140</v>
+        <v>30</v>
       </c>
       <c r="E82" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="83" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C83" t="s">
+        <v>59</v>
+      </c>
+      <c r="D83">
+        <v>140</v>
+      </c>
+      <c r="E83" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
         <v>60</v>
       </c>
-      <c r="D83">
-        <f>D82*1000/(PI()*D81)</f>
+      <c r="D84">
+        <f>D83*1000/(PI()*D82)</f>
         <v>1485.4461355243566</v>
       </c>
-      <c r="E83" t="s">
+      <c r="E84" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="85" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C85" t="s">
+    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
         <v>62</v>
       </c>
-      <c r="D85">
+      <c r="D86">
         <v>0.1</v>
       </c>
-      <c r="E85" t="s">
+      <c r="E86" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="87" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C87" t="s">
+    <row r="88" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
         <v>67</v>
       </c>
-      <c r="D87">
-        <f>D85*D83</f>
+      <c r="D88">
+        <f>D86*D84</f>
         <v>148.54461355243566</v>
       </c>
-      <c r="E87" t="s">
+      <c r="E88" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- DOC fix for cycle_ID_turning - feed calculation now respects max RPM setting - M0 added to cycle_ID_turning
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Koen\Projecten\Emcoturn 120\edingCNC\cnc_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC75677B-D2A0-4ECB-88FF-FF6521A10FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F976FF39-B388-4916-89DB-DE22F5398E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
   <si>
     <t>EdingCNC variables</t>
   </si>
@@ -128,9 +128,6 @@
     <t>Return value for dlgmsg  1=OK, -1=cancel</t>
   </si>
   <si>
-    <t>simple_turning</t>
-  </si>
-  <si>
     <t>Z1</t>
   </si>
   <si>
@@ -258,6 +255,15 @@
   </si>
   <si>
     <t>rpm calculation</t>
+  </si>
+  <si>
+    <t>F, feed per rev [mm/rev]</t>
+  </si>
+  <si>
+    <t>cycle_ID_turning</t>
+  </si>
+  <si>
+    <t>cycle_OD_turning</t>
   </si>
 </sst>
 </file>
@@ -608,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,10 +683,10 @@
         <v>1400</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D8" s="7"/>
     </row>
@@ -689,10 +695,10 @@
         <v>1401</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -701,10 +707,10 @@
         <v>1402</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D10" s="7"/>
     </row>
@@ -713,10 +719,10 @@
         <v>1403</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D11" s="7"/>
     </row>
@@ -725,10 +731,10 @@
         <v>1404</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D12" s="7"/>
     </row>
@@ -737,10 +743,10 @@
         <v>1405</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D13" s="7"/>
     </row>
@@ -749,10 +755,10 @@
         <v>1406</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D14" s="7"/>
     </row>
@@ -761,10 +767,10 @@
         <v>1407</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D15" s="7"/>
     </row>
@@ -773,10 +779,10 @@
         <v>1408</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D16" s="7"/>
     </row>
@@ -785,10 +791,10 @@
         <v>1409</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D17" s="7"/>
     </row>
@@ -797,10 +803,10 @@
         <v>1410</v>
       </c>
       <c r="B18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D18" s="7"/>
     </row>
@@ -809,10 +815,10 @@
         <v>1411</v>
       </c>
       <c r="B19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D19" s="7"/>
     </row>
@@ -821,10 +827,10 @@
         <v>1412</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>27</v>
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
       </c>
       <c r="D20" s="7"/>
     </row>
@@ -833,10 +839,10 @@
         <v>1413</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>27</v>
+        <v>56</v>
+      </c>
+      <c r="C21" t="s">
+        <v>72</v>
       </c>
       <c r="D21" s="7"/>
     </row>
@@ -845,10 +851,10 @@
         <v>1414</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="D22" s="7"/>
     </row>
@@ -857,10 +863,10 @@
         <v>1450</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D23" s="7"/>
     </row>
@@ -869,10 +875,10 @@
         <v>1451</v>
       </c>
       <c r="B24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D24" s="7"/>
     </row>
@@ -881,10 +887,10 @@
         <v>1452</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D25" s="7"/>
     </row>
@@ -893,10 +899,10 @@
         <v>1453</v>
       </c>
       <c r="B26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D26" s="7"/>
     </row>
@@ -905,10 +911,10 @@
         <v>1454</v>
       </c>
       <c r="B27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D27" s="7"/>
     </row>
@@ -917,10 +923,10 @@
         <v>1455</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D28" s="7"/>
     </row>
@@ -929,10 +935,10 @@
         <v>1456</v>
       </c>
       <c r="B29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D29" s="7"/>
     </row>
@@ -941,10 +947,10 @@
         <v>1457</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D30" s="7"/>
     </row>
@@ -953,10 +959,10 @@
         <v>1458</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D31" s="7"/>
     </row>
@@ -965,10 +971,10 @@
         <v>1459</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D32" s="7"/>
     </row>
@@ -977,10 +983,10 @@
         <v>1460</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D33" s="7"/>
     </row>
@@ -989,10 +995,10 @@
         <v>1461</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D34" s="7"/>
     </row>
@@ -1001,10 +1007,10 @@
         <v>1462</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="7"/>
     </row>
@@ -1013,10 +1019,10 @@
         <v>1463</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D36" s="7"/>
     </row>
@@ -1025,10 +1031,10 @@
         <v>1500</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" s="7"/>
     </row>
@@ -1037,10 +1043,10 @@
         <v>1501</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1048,10 +1054,10 @@
         <v>1502</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,10 +1065,10 @@
         <v>1503</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1070,10 +1076,10 @@
         <v>1504</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C41" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1081,10 +1087,10 @@
         <v>1505</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1092,10 +1098,10 @@
         <v>1506</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1103,10 +1109,10 @@
         <v>1507</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1114,10 +1120,10 @@
         <v>1508</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1125,10 +1131,10 @@
         <v>1509</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1136,10 +1142,10 @@
         <v>1510</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1147,10 +1153,10 @@
         <v>1511</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C48" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1158,10 +1164,10 @@
         <v>1512</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
@@ -1170,7 +1176,7 @@
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1179,7 +1185,7 @@
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
@@ -1188,7 +1194,7 @@
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1197,7 +1203,7 @@
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -1206,7 +1212,7 @@
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
@@ -1215,7 +1221,7 @@
       </c>
       <c r="B55" s="8"/>
       <c r="C55" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
@@ -1223,214 +1229,410 @@
         <v>1556</v>
       </c>
       <c r="C56" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="5">
+        <v>1557</v>
+      </c>
+      <c r="B57" s="6"/>
+      <c r="C57" s="9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="10">
+        <v>1600</v>
+      </c>
+      <c r="B58" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="10">
+        <v>1601</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="10">
+        <v>1602</v>
+      </c>
+      <c r="B60" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="10">
+        <v>1603</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="10">
+        <v>1604</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="10">
+        <v>1605</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="10">
+        <v>1606</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="10">
+        <v>1607</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C65" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="10">
+        <v>1608</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="10">
+        <v>1609</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="10">
+        <v>1610</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C68" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="10">
+        <v>1611</v>
+      </c>
+      <c r="B69" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C69" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="10">
+        <v>1612</v>
+      </c>
+      <c r="B70" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C70" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="10">
+        <v>1613</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="10">
+        <v>1614</v>
+      </c>
+      <c r="B72" s="8" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="10">
-        <v>1557</v>
-      </c>
-      <c r="C57" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="4"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="3">
+      <c r="C72" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="10"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="8"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="10"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="10"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="8"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="10"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="8"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="10"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="8"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="10"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="8"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="4"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="4"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="4"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
         <v>5001</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B82" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
         <v>5002</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B83" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
         <v>5003</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B84" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
         <v>5004</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B85" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
         <v>5005</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B86" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="3">
         <v>5006</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B87" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
         <v>5008</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B88" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="3">
         <v>5009</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B89" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="3">
         <v>5010</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B90" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="3">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
         <v>5011</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B91" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
         <v>5012</v>
       </c>
-      <c r="B71" t="s">
+      <c r="B92" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="3">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
         <v>5013</v>
       </c>
-      <c r="B72" t="s">
+      <c r="B93" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="3">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
         <v>5009</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B94" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>18</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B96" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97" s="3">
         <v>5380</v>
       </c>
-      <c r="B76" t="s">
+      <c r="B97" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98" s="3">
         <v>5398</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B98" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>57</v>
+      </c>
+      <c r="D103">
+        <v>30</v>
+      </c>
+      <c r="E103" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>58</v>
+      </c>
+      <c r="D104">
+        <v>140</v>
+      </c>
+      <c r="E104" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>59</v>
+      </c>
+      <c r="D105">
+        <f>D104*1000/(PI()*D103)</f>
+        <v>1485.4461355243566</v>
+      </c>
+      <c r="E105" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C82" t="s">
-        <v>58</v>
-      </c>
-      <c r="D82">
-        <v>30</v>
-      </c>
-      <c r="E82" t="s">
+      <c r="D107">
+        <v>0.1</v>
+      </c>
+      <c r="E107" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C83" t="s">
-        <v>59</v>
-      </c>
-      <c r="D83">
-        <v>140</v>
-      </c>
-      <c r="E83" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C84" t="s">
-        <v>60</v>
-      </c>
-      <c r="D84">
-        <f>D83*1000/(PI()*D82)</f>
-        <v>1485.4461355243566</v>
-      </c>
-      <c r="E84" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="86" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C86" t="s">
-        <v>62</v>
-      </c>
-      <c r="D86">
-        <v>0.1</v>
-      </c>
-      <c r="E86" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="88" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C88" t="s">
+      <c r="D109">
+        <f>D107*D105</f>
+        <v>148.54461355243566</v>
+      </c>
+      <c r="E109" t="s">
         <v>67</v>
-      </c>
-      <c r="D88">
-        <f>D86*D84</f>
-        <v>148.54461355243566</v>
-      </c>
-      <c r="E88" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update to drilling cycle: - default drill diameter is actual tool diameter - feed to 0% before movements - end of cycle retract Z, then X up
</commit_message>
<xml_diff>
--- a/variables.xlsx
+++ b/variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Koen\Projecten\Emcoturn 120\edingCNC\cnc_config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F976FF39-B388-4916-89DB-DE22F5398E61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4299B25A-9FC8-4D73-8489-DC6CD5A49BA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2205" yWindow="2205" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="86">
   <si>
     <t>EdingCNC variables</t>
   </si>
@@ -264,6 +264,45 @@
   </si>
   <si>
     <t>cycle_OD_turning</t>
+  </si>
+  <si>
+    <t>cycle_parting_off</t>
+  </si>
+  <si>
+    <t>Zstart</t>
+  </si>
+  <si>
+    <t>tool width</t>
+  </si>
+  <si>
+    <t>feed per rev</t>
+  </si>
+  <si>
+    <t>spindle speed</t>
+  </si>
+  <si>
+    <t>pecking depth</t>
+  </si>
+  <si>
+    <t>dwell time</t>
+  </si>
+  <si>
+    <t>pitch</t>
+  </si>
+  <si>
+    <t>depth per pass</t>
+  </si>
+  <si>
+    <t>spindle speed rev/min</t>
+  </si>
+  <si>
+    <t>full thread depth beyond thread peak</t>
+  </si>
+  <si>
+    <t>cycle_internal_threading</t>
+  </si>
+  <si>
+    <t>cycle_OD_turning_chamfer_radius</t>
   </si>
 </sst>
 </file>
@@ -614,10 +653,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1395,243 +1434,498 @@
         <v>71</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="10">
+    <row r="72" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="5">
         <v>1614</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="B72" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C72" s="8" t="s">
+      <c r="C72" s="9" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="10"/>
-      <c r="B73" s="7"/>
-      <c r="C73" s="8"/>
+      <c r="A73" s="10">
+        <v>1650</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="10"/>
-      <c r="B74" s="7"/>
-      <c r="C74" s="8"/>
+      <c r="A74" s="10">
+        <v>1651</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C74" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="10"/>
-      <c r="B75" s="7"/>
-      <c r="C75" s="8"/>
+      <c r="A75" s="10">
+        <v>1652</v>
+      </c>
+      <c r="B75" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C75" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="10"/>
-      <c r="B76" s="7"/>
-      <c r="C76" s="8"/>
+      <c r="A76" s="10">
+        <v>1653</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C76" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="10"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="8"/>
+      <c r="A77" s="10">
+        <v>1654</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="10"/>
-      <c r="B78" s="7"/>
-      <c r="C78" s="8"/>
+      <c r="A78" s="10">
+        <v>1655</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C78" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="4"/>
+      <c r="A79" s="4">
+        <v>1656</v>
+      </c>
+      <c r="B79" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C79" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="4"/>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="4"/>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="3">
+      <c r="A80" s="4">
+        <v>1657</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="5">
+        <v>1658</v>
+      </c>
+      <c r="B81" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C81" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="10">
+        <v>1700</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C82" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="10">
+        <v>1701</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C83" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="10">
+        <v>1702</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C84" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="10">
+        <v>1703</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C85" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="10">
+        <v>1704</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C86" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="10">
+        <v>1705</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="C87" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="10">
+        <v>1706</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="10">
+        <v>1707</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C89" s="8" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="5">
+        <v>1708</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C90" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="10">
+        <v>1750</v>
+      </c>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="10"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="10"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="10"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="10"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="10"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="10"/>
+      <c r="B97" s="8"/>
+      <c r="C97" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="10"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="10"/>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="10"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="10"/>
+      <c r="B101" s="8"/>
+      <c r="C101" s="8"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="10"/>
+      <c r="B102" s="8"/>
+      <c r="C102" s="8"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="10"/>
+      <c r="B103" s="8"/>
+      <c r="C103" s="8"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="10"/>
+      <c r="B104" s="8"/>
+      <c r="C104" s="8"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="10"/>
+      <c r="B105" s="8"/>
+      <c r="C105" s="8"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="4"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="3">
         <v>5001</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B107" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="3">
         <v>5002</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B108" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="3">
         <v>5003</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B109" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="3">
         <v>5004</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B110" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="3">
         <v>5005</v>
       </c>
-      <c r="B86" t="s">
+      <c r="B111" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="3">
         <v>5006</v>
       </c>
-      <c r="B87" t="s">
+      <c r="B112" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" s="3">
         <v>5008</v>
       </c>
-      <c r="B88" t="s">
+      <c r="B113" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
         <v>5009</v>
       </c>
-      <c r="B89" t="s">
+      <c r="B114" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" s="3">
         <v>5010</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B115" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116" s="3">
         <v>5011</v>
       </c>
-      <c r="B91" t="s">
+      <c r="B116" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" s="3">
         <v>5012</v>
       </c>
-      <c r="B92" t="s">
+      <c r="B117" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118" s="3">
         <v>5013</v>
       </c>
-      <c r="B93" t="s">
+      <c r="B118" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119" s="3">
         <v>5009</v>
       </c>
-      <c r="B94" t="s">
+      <c r="B119" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>18</v>
       </c>
-      <c r="B96" t="s">
+      <c r="B121" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A97" s="3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122" s="3">
         <v>5380</v>
       </c>
-      <c r="B97" t="s">
+      <c r="B122" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A98" s="3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123" s="3">
         <v>5398</v>
       </c>
-      <c r="B98" t="s">
+      <c r="B123" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C100" t="s">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C125" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C103" t="s">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C128" t="s">
         <v>57</v>
       </c>
-      <c r="D103">
+      <c r="D128">
         <v>30</v>
       </c>
-      <c r="E103" t="s">
+      <c r="E128" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C104" t="s">
+    <row r="129" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C129" t="s">
         <v>58</v>
       </c>
-      <c r="D104">
+      <c r="D129">
         <v>140</v>
       </c>
-      <c r="E104" t="s">
+      <c r="E129" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C105" t="s">
+    <row r="130" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C130" t="s">
         <v>59</v>
       </c>
-      <c r="D105">
-        <f>D104*1000/(PI()*D103)</f>
+      <c r="D130">
+        <f>D129*1000/(PI()*D128)</f>
         <v>1485.4461355243566</v>
       </c>
-      <c r="E105" t="s">
+      <c r="E130" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C107" t="s">
+    <row r="132" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C132" t="s">
         <v>61</v>
       </c>
-      <c r="D107">
+      <c r="D132">
         <v>0.1</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E132" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C109" t="s">
+    <row r="134" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
         <v>66</v>
       </c>
-      <c r="D109">
-        <f>D107*D105</f>
+      <c r="D134">
+        <f>D132*D130</f>
         <v>148.54461355243566</v>
       </c>
-      <c r="E109" t="s">
+      <c r="E134" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>